<commit_message>
many updates, set up the repo
</commit_message>
<xml_diff>
--- a/data/raw_data/elisa 17.11 results.xlsx
+++ b/data/raw_data/elisa 17.11 results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matan\Desktop\stubility\insulin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PhD\pythonProject_model_improvement\code_repo\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BB597C-C0CB-445E-BD0F-AA9772A98344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159B9B7F-353C-4294-9C13-9A8D6E63AC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
@@ -1570,6 +1570,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1577,7 +1578,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1747,22 +1747,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1919,22 +1919,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2091,22 +2091,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2263,22 +2263,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6408,20 +6408,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:T112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K103" sqref="K103"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="12" max="12" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6429,7 +6429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -6437,12 +6437,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>44882</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -6466,7 +6466,7 @@
         <v>0.58288194444444441</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -6482,7 +6482,7 @@
         <v>18111919</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -6490,13 +6490,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -6504,12 +6504,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -6517,28 +6517,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="4"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="6">
         <v>1</v>
@@ -6585,7 +6585,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>25</v>
       </c>
@@ -6611,7 +6611,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>26</v>
       </c>
@@ -6637,7 +6637,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>27</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>28</v>
       </c>
@@ -6691,7 +6691,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
         <v>29</v>
       </c>
@@ -6719,7 +6719,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
         <v>30</v>
       </c>
@@ -6747,7 +6747,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>31</v>
       </c>
@@ -6775,7 +6775,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>32</v>
       </c>
@@ -6801,7 +6801,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="38" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>560</v>
       </c>
@@ -6834,7 +6834,7 @@
         <v>9.6096096096096095E-2</v>
       </c>
     </row>
-    <row r="39" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D39">
         <f t="shared" si="0"/>
         <v>2.1366366366366365</v>
@@ -6864,7 +6864,7 @@
         <v>0.28978978978978981</v>
       </c>
     </row>
-    <row r="41" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D41">
         <f>D38*1120</f>
         <v>2154.234234234234</v>
@@ -6915,7 +6915,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="42" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
       <c r="M42" s="12">
         <v>1.423</v>
       </c>
@@ -6938,7 +6938,7 @@
         <v>0.193</v>
       </c>
     </row>
-    <row r="43" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>45</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>22.416336443664452</v>
       </c>
     </row>
-    <row r="44" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>35</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>107.627</v>
       </c>
     </row>
-    <row r="45" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D45">
         <v>1975.721</v>
       </c>
@@ -7020,7 +7020,7 @@
         <v>160.32900000000001</v>
       </c>
     </row>
-    <row r="46" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D46">
         <v>2201.9430000000002</v>
       </c>
@@ -7043,7 +7043,7 @@
         <v>147.32300000000001</v>
       </c>
     </row>
-    <row r="47" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>41</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="3:19" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>45</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>36</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D50">
         <v>2531.098</v>
       </c>
@@ -7172,7 +7172,7 @@
         <v>2.2034964441554641E-2</v>
       </c>
     </row>
-    <row r="51" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D51">
         <v>2240.9870000000001</v>
       </c>
@@ -7216,7 +7216,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>40</v>
       </c>
@@ -7249,7 +7249,7 @@
         <v>328.56726666666668</v>
       </c>
     </row>
-    <row r="53" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
       <c r="N53">
         <v>2110.6326666666669</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>138.42633333333333</v>
       </c>
     </row>
-    <row r="54" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>45</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>328.56726666666668</v>
       </c>
     </row>
-    <row r="55" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>37</v>
       </c>
@@ -7377,7 +7377,7 @@
         <v>1990.0596666666668</v>
       </c>
     </row>
-    <row r="56" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D56">
         <v>2893.4630000000002</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>1937.4750000000001</v>
       </c>
     </row>
-    <row r="57" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D57">
         <v>2932.3429999999998</v>
       </c>
@@ -7465,7 +7465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D58">
         <f>AVERAGE(D55:D57)</f>
         <v>2852.9296666666669</v>
@@ -7499,7 +7499,7 @@
         <v>1.0811292863626576E-9</v>
       </c>
     </row>
-    <row r="59" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>45</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v>49.413551629757045</v>
       </c>
     </row>
-    <row r="60" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>38</v>
       </c>
@@ -7558,7 +7558,7 @@
         <v>1969.058</v>
       </c>
     </row>
-    <row r="61" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D61">
         <v>2553.7930000000001</v>
       </c>
@@ -7596,7 +7596,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="62" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D62">
         <v>2633.8719999999998</v>
       </c>
@@ -7619,7 +7619,7 @@
         <v>1867.6980000000001</v>
       </c>
     </row>
-    <row r="63" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D63">
         <f>AVERAGE(D60:D62)</f>
         <v>2546.7443333333335</v>
@@ -7649,7 +7649,7 @@
         <v>1937.4750000000001</v>
       </c>
     </row>
-    <row r="64" spans="3:20" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>45</v>
       </c>
@@ -7682,7 +7682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
         <v>39</v>
       </c>
@@ -7708,7 +7708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D66">
         <v>1083.424</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D67">
         <v>1124.3889999999999</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D68">
         <f>AVERAGE(D65:D67)</f>
         <v>1137.1193333333333</v>
@@ -7784,7 +7784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>48</v>
       </c>
@@ -7798,7 +7798,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
         <v>47</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D72">
         <v>2110.6326666666669</v>
       </c>
@@ -7837,7 +7837,7 @@
         <v>1.3516940734042147</v>
       </c>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D73">
         <v>1</v>
       </c>
@@ -7846,7 +7846,7 @@
         <v>1.2066260385116754</v>
       </c>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D74">
         <v>2154.2339999999999</v>
       </c>
@@ -7869,7 +7869,7 @@
         <v>1.2948643518894334</v>
       </c>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D75">
         <v>1975.721</v>
       </c>
@@ -7892,7 +7892,7 @@
         <v>1.3708984257169019</v>
       </c>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D76">
         <v>2201.9430000000002</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>1.3893194426063085</v>
       </c>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E78">
         <f>_xlfn.T.TEST(E74:E76,H74:H76,1,2)</f>
         <v>3.6446490905162388E-3</v>
@@ -7925,7 +7925,7 @@
         <v>6.406533194727314E-4</v>
       </c>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>51</v>
       </c>
@@ -7945,7 +7945,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>0</v>
       </c>
@@ -7965,7 +7965,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C84">
         <v>2.8</v>
       </c>
@@ -7982,30 +7982,30 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C87">
         <v>0</v>
       </c>
       <c r="D87">
+        <v>5</v>
+      </c>
+      <c r="E87">
         <v>10</v>
       </c>
-      <c r="E87">
+      <c r="F87">
         <v>15</v>
       </c>
-      <c r="F87">
+      <c r="G87">
         <v>20</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>25</v>
       </c>
-      <c r="H87">
+      <c r="I87">
         <v>30</v>
       </c>
-      <c r="I87">
-        <v>35</v>
-      </c>
     </row>
-    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C88">
         <v>73</v>
       </c>
@@ -8028,7 +8028,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="89" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C89">
         <v>81</v>
       </c>
@@ -8051,7 +8051,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C90">
         <v>89</v>
       </c>
@@ -8074,7 +8074,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C91">
         <v>102</v>
       </c>
@@ -8097,7 +8097,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C93" s="21" t="s">
         <v>51</v>
       </c>
@@ -8111,7 +8111,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="97" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C97">
         <v>5</v>
       </c>
@@ -8140,7 +8140,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="98" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C98">
         <v>4.9000000000000004</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="99" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C99">
         <v>5.6</v>
       </c>
@@ -8198,7 +8198,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="100" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C100">
         <v>5.8</v>
       </c>
@@ -8227,7 +8227,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="105" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C105">
         <v>0</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C106">
         <v>102</v>
       </c>
@@ -8291,7 +8291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C107">
         <v>98</v>
       </c>
@@ -8323,7 +8323,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="108" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C108">
         <v>83</v>
       </c>
@@ -8355,7 +8355,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="109" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C109">
         <v>105</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="112" spans="3:12" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D112" s="21" t="s">
         <v>56</v>
       </c>
@@ -8416,7 +8416,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>